<commit_message>
places added, rnadomization started doubleconstructure not that good
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Enemies.xlsx
+++ b/OpenWorld/Resources/Enemies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>agressivity</t>
+  </si>
+  <si>
+    <t>Troll</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="G1:I3"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +740,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
just not to lose anything
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Enemies.xlsx
+++ b/OpenWorld/Resources/Enemies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Troll</t>
+  </si>
+  <si>
+    <t>Bandit</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +763,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
enemies extended, bug fixed where running makes you look like you wanted to wait
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Enemies.xlsx
+++ b/OpenWorld/Resources/Enemies.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2D6F7B-FBD6-4102-A1A2-60F845E31DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017219D4-B768-4492-8E16-01E161669167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -537,18 +537,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -630,7 +630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -670,7 +670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -690,7 +690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -710,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -730,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -770,7 +770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -790,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -830,7 +830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -870,7 +870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -890,124 +890,484 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
+      </c>
+      <c r="B41">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>